<commit_message>
Updated Utility component to fetch UNC path dynamically from config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CoEDevelopmentBotVPe\Documents\Configuration\Dispatcher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev2Mercury\Documents\UiPath\InPwr.Finance.AccountsPayable.Common.Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AD1620-E62D-4156-AABD-70C4AA0EBA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97290000-C429-4D4E-8B8D-548961B9D091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -286,9 +286,6 @@
     <t>AP_SharedDrive_UNC</t>
   </si>
   <si>
-    <t>\\inpwrautomation.file.core.windows.net\automation\</t>
-  </si>
-  <si>
     <t>Actual share drive path and IP address are not allowed.</t>
   </si>
   <si>
@@ -365,6 +362,9 @@
   </si>
   <si>
     <t>Business Exception Occurred</t>
+  </si>
+  <si>
+    <t>\\automationsvr\automation</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -474,7 +474,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -795,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y970"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -845,7 +844,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>60</v>
@@ -856,7 +855,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>67</v>
@@ -882,7 +881,7 @@
         <v>69</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>59</v>
@@ -937,10 +936,10 @@
     </row>
     <row r="13" spans="1:25" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="14.25" customHeight="1">
@@ -955,29 +954,29 @@
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="14.25" customHeight="1">
       <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
@@ -985,10 +984,10 @@
         <v>84</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
@@ -1018,10 +1017,10 @@
         <v>76</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -1029,7 +1028,7 @@
         <v>77</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>66</v>
@@ -1043,7 +1042,7 @@
         <v>63</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
@@ -3227,7 +3226,7 @@
         <v>70</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -3241,10 +3240,10 @@
         <v>82</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3255,7 +3254,7 @@
         <v>69</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>59</v>
@@ -4243,8 +4242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A045ED-89B2-46F5-87BB-9D73B35EE197}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4281,31 +4280,31 @@
       <c r="B2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>106</v>
+      <c r="C2" t="s">
+        <v>105</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>52</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="240">
+      <c r="A3" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="240">
-      <c r="A3" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>109</v>
-      </c>
       <c r="E3" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -4361,7 +4360,7 @@
         <v>51</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>50</v>

</xml_diff>